<commit_message>
commit at 12 51
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\utksi\Downloads\DAA Webpage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F3E137-8CB8-4B28-8254-F5904B6EED8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1694B222-611D-4D2E-BCAE-5E765CA7C7FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{1CA7FFA8-CD19-4F3B-B2CA-E99C1209A65C}"/>
   </bookViews>
@@ -20,17 +20,6 @@
     <sheet name="Khush Wiki" sheetId="4" r:id="rId5"/>
     <sheet name="Khush Enron" sheetId="5" r:id="rId6"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Daksh Enron'!$A$2:$A$20</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Daksh Enron'!$B$1</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Daksh Enron'!$B$2:$B$20</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Daksh Enron'!$A$2:$A$20</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'Daksh Enron'!$B$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'Daksh Enron'!$B$2:$B$20</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'Daksh Enron'!$A$2:$A$20</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'Daksh Enron'!$B$1</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'Daksh Enron'!$B$2:$B$20</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -50,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="7">
   <si>
     <t>Size</t>
   </si>
@@ -1929,7 +1918,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.43852200000000002</c:v>
+                  <c:v>0.51500000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1983,7 +1972,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1.2318100000000001</c:v>
+                  <c:v>1.6659999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2037,7 +2026,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>3351.14</c:v>
+                  <c:v>4674.17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2351,6 +2340,64 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:numRef>
               <c:f>'Khush Wiki'!$A$2:$A$17</c:f>
@@ -2415,52 +2462,52 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>8655</c:v>
+                  <c:v>14070</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13718</c:v>
+                  <c:v>7077</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27292</c:v>
+                  <c:v>13319</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>48416</c:v>
+                  <c:v>18143</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>68872</c:v>
+                  <c:v>22715</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>83266</c:v>
+                  <c:v>25896</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>76732</c:v>
+                  <c:v>24766</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>54456</c:v>
+                  <c:v>22884</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>35470</c:v>
+                  <c:v>21393</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>21736</c:v>
+                  <c:v>17833</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11640</c:v>
+                  <c:v>15181</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5449</c:v>
+                  <c:v>11487</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2329</c:v>
+                  <c:v>7417</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>740</c:v>
+                  <c:v>3157</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>208</c:v>
+                  <c:v>1178</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>23</c:v>
+                  <c:v>286</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2472,8 +2519,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -6417,16 +6465,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>68580</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>110490</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>140970</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>373380</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>110490</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>26670</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6458,16 +6506,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>396240</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>41910</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>3810</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>91440</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>41910</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7721,10 +7769,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7578E71D-AE83-4834-9183-06E518800F42}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7745,7 +7793,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="2">
-        <v>0.43852200000000002</v>
+        <v>0.51500000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -7753,7 +7801,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="2">
-        <v>1.2318100000000001</v>
+        <v>1.6659999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -7761,7 +7809,39 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>3351.14</v>
+        <v>4674.17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.51500000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1.6659999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="2">
+        <v>4674.17</v>
       </c>
     </row>
   </sheetData>
@@ -7774,8 +7854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E99B00E-D41B-4389-89BE-A60AB9B57575}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView topLeftCell="B6" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7793,7 +7873,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>8655</v>
+        <v>14070</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -7801,7 +7881,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>13718</v>
+        <v>7077</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -7809,7 +7889,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>27292</v>
+        <v>13319</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -7817,7 +7897,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>48416</v>
+        <v>18143</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -7825,7 +7905,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>68872</v>
+        <v>22715</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -7833,7 +7913,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>83266</v>
+        <v>25896</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -7841,7 +7921,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>76732</v>
+        <v>24766</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -7849,7 +7929,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>54456</v>
+        <v>22884</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -7857,7 +7937,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>35470</v>
+        <v>21393</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -7865,7 +7945,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>21736</v>
+        <v>17833</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -7873,7 +7953,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>11640</v>
+        <v>15181</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -7881,7 +7961,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>5449</v>
+        <v>11487</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -7889,7 +7969,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>2329</v>
+        <v>7417</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -7897,7 +7977,7 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>740</v>
+        <v>3157</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -7905,7 +7985,7 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>208</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -7913,7 +7993,7 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <v>23</v>
+        <v>286</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit at 01 05
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\utksi\Downloads\DAA Webpage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1694B222-611D-4D2E-BCAE-5E765CA7C7FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{936DF3A8-74F5-4BD4-8033-6397AF09749E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{1CA7FFA8-CD19-4F3B-B2CA-E99C1209A65C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{1CA7FFA8-CD19-4F3B-B2CA-E99C1209A65C}"/>
   </bookViews>
   <sheets>
     <sheet name="Daksh Wiki" sheetId="1" r:id="rId1"/>
     <sheet name="Daksh Enron" sheetId="2" r:id="rId2"/>
     <sheet name="Daksh Skitter" sheetId="3" r:id="rId3"/>
     <sheet name="Daksh Hist" sheetId="6" r:id="rId4"/>
-    <sheet name="Khush Wiki" sheetId="4" r:id="rId5"/>
-    <sheet name="Khush Enron" sheetId="5" r:id="rId6"/>
+    <sheet name="Khush Skitter" sheetId="7" r:id="rId5"/>
+    <sheet name="Khush Wiki" sheetId="4" r:id="rId6"/>
+    <sheet name="Khush Enron" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="7">
   <si>
     <t>Size</t>
   </si>
@@ -2254,6 +2255,695 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Khush Skitter'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Number of Cliques</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Khush Skitter'!$A$2:$A$67</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="66"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>67</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Khush Skitter'!$B$2:$B$67</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="66"/>
+                <c:pt idx="0">
+                  <c:v>2319807</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3171609</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1823321</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>939336</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>684873</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>598284</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>588889</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>608937</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>665661</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>728098</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>798073</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>877282</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>945194</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>980831</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>939987</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>839330</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>729601</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>639413</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>600192</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>611976</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>640890</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>673924</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>706753</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>753633</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>818353</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>892719</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>955212</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>999860</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1034106</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1055653</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1017560</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>946717</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>878552</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>809485</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>744634</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>663650</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>583922</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>520239</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>474301</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>420796</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>367879</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>321829</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>275995</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>222461</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>158352</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>99522</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>62437</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>39822</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>30011</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>25637</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>17707</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>9514</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>3737</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2042</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1080</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>546</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>449</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>447</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>405</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>283</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>242</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AA7C-4907-BF95-01BB3EA80244}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="161908832"/>
+        <c:axId val="161919392"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="161908832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="161919392"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="161919392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="161908832"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
     <c:title>
       <c:tx>
         <c:rich>
@@ -2684,7 +3374,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3327,6 +4017,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
@@ -5836,6 +6566,509 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6506,6 +7739,49 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>33020</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1270</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>43</xdr:col>
+      <xdr:colOff>337820</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>1270</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5796DFB6-843F-D31B-9908-604A612E2E88}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noChangeAspect="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
@@ -6543,7 +7819,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -7771,7 +9047,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7578E71D-AE83-4834-9183-06E518800F42}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -7851,6 +9127,558 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F1AB2EC-9B94-4E5C-9219-C96B9719F573}">
+  <dimension ref="A1:B67"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R57" sqref="R57"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>2319807</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>3171609</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>1823321</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>939336</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>684873</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>598284</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>588889</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>608937</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>665661</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>728098</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>798073</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>877282</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>945194</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>980831</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>939987</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>839330</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>729601</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>639413</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>600192</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>611976</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>22</v>
+      </c>
+      <c r="B22">
+        <v>640890</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>23</v>
+      </c>
+      <c r="B23">
+        <v>673924</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>24</v>
+      </c>
+      <c r="B24">
+        <v>706753</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>25</v>
+      </c>
+      <c r="B25">
+        <v>753633</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>26</v>
+      </c>
+      <c r="B26">
+        <v>818353</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>27</v>
+      </c>
+      <c r="B27">
+        <v>892719</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>28</v>
+      </c>
+      <c r="B28">
+        <v>955212</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>29</v>
+      </c>
+      <c r="B29">
+        <v>999860</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>30</v>
+      </c>
+      <c r="B30">
+        <v>1034106</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>31</v>
+      </c>
+      <c r="B31">
+        <v>1055653</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>32</v>
+      </c>
+      <c r="B32">
+        <v>1017560</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>33</v>
+      </c>
+      <c r="B33">
+        <v>946717</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>34</v>
+      </c>
+      <c r="B34">
+        <v>878552</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>35</v>
+      </c>
+      <c r="B35">
+        <v>809485</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>36</v>
+      </c>
+      <c r="B36">
+        <v>744634</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>37</v>
+      </c>
+      <c r="B37">
+        <v>663650</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>38</v>
+      </c>
+      <c r="B38">
+        <v>583922</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>39</v>
+      </c>
+      <c r="B39">
+        <v>520239</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>40</v>
+      </c>
+      <c r="B40">
+        <v>474301</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>41</v>
+      </c>
+      <c r="B41">
+        <v>420796</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>42</v>
+      </c>
+      <c r="B42">
+        <v>367879</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>43</v>
+      </c>
+      <c r="B43">
+        <v>321829</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>44</v>
+      </c>
+      <c r="B44">
+        <v>275995</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>45</v>
+      </c>
+      <c r="B45">
+        <v>222461</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>46</v>
+      </c>
+      <c r="B46">
+        <v>158352</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>47</v>
+      </c>
+      <c r="B47">
+        <v>99522</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>48</v>
+      </c>
+      <c r="B48">
+        <v>62437</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>49</v>
+      </c>
+      <c r="B49">
+        <v>39822</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>50</v>
+      </c>
+      <c r="B50">
+        <v>30011</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>51</v>
+      </c>
+      <c r="B51">
+        <v>25637</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>52</v>
+      </c>
+      <c r="B52">
+        <v>17707</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>53</v>
+      </c>
+      <c r="B53">
+        <v>9514</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>54</v>
+      </c>
+      <c r="B54">
+        <v>3737</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>55</v>
+      </c>
+      <c r="B55">
+        <v>2042</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>56</v>
+      </c>
+      <c r="B56">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>57</v>
+      </c>
+      <c r="B57">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>58</v>
+      </c>
+      <c r="B58">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>59</v>
+      </c>
+      <c r="B59">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>60</v>
+      </c>
+      <c r="B60">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>61</v>
+      </c>
+      <c r="B61">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>62</v>
+      </c>
+      <c r="B62">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>63</v>
+      </c>
+      <c r="B63">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>64</v>
+      </c>
+      <c r="B64">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>65</v>
+      </c>
+      <c r="B65">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>66</v>
+      </c>
+      <c r="B66">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>67</v>
+      </c>
+      <c r="B67">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E99B00E-D41B-4389-89BE-A60AB9B57575}">
   <dimension ref="A1:B17"/>
   <sheetViews>
@@ -8002,7 +9830,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26B5ADBC-C9CD-4AA4-8451-2A40CE7C2F85}">
   <dimension ref="A1:B20"/>
   <sheetViews>

</xml_diff>